<commit_message>
New SDM port data
</commit_message>
<xml_diff>
--- a/Data/Ports/port_coord.xlsx
+++ b/Data/Ports/port_coord.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\EconAnalysis\Data\Ports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77B639E8-23E2-4C39-B508-82272A6CC9CF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD91239D-AAB6-4588-89DA-3D203E30551E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="70">
   <si>
     <t>port_name</t>
   </si>
@@ -209,6 +209,27 @@
   </si>
   <si>
     <t>WHIDBY ISLAND</t>
+  </si>
+  <si>
+    <t>CHINOOK</t>
+  </si>
+  <si>
+    <t>FIELDS LANDING</t>
+  </si>
+  <si>
+    <t>GUADALUPE</t>
+  </si>
+  <si>
+    <t>MARCONI</t>
+  </si>
+  <si>
+    <t>PORT ORFORD</t>
+  </si>
+  <si>
+    <t>VALLEJO</t>
+  </si>
+  <si>
+    <t>WILLOW CREEK</t>
   </si>
 </sst>
 </file>
@@ -1056,20 +1077,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C61"/>
+  <dimension ref="A1:C68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="A56" sqref="A56"/>
+    <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
+      <selection activeCell="F54" sqref="F54"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="26.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1080,7 +1101,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -1091,7 +1112,7 @@
         <v>-121.891876</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -1102,7 +1123,7 @@
         <v>-121.79007799999999</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -1113,7 +1134,7 @@
         <v>-117.401141</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -1124,7 +1145,7 @@
         <v>-119.22840100000001</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -1135,7 +1156,7 @@
         <v>-119.21339399999999</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -1146,7 +1167,7 @@
         <v>-118.259165</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -1157,7 +1178,7 @@
         <v>-122.00117899999999</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>10</v>
       </c>
@@ -1168,7 +1189,7 @@
         <v>-118.249824</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>11</v>
       </c>
@@ -1179,7 +1200,7 @@
         <v>-119.68592</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>12</v>
       </c>
@@ -1190,7 +1211,7 @@
         <v>-117.26029200000001</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>13</v>
       </c>
@@ -1201,7 +1222,7 @@
         <v>-117.878085</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>14</v>
       </c>
@@ -1212,7 +1233,7 @@
         <v>-122.47671099999999</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>15</v>
       </c>
@@ -1223,7 +1244,7 @@
         <v>-118.10122800000001</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>16</v>
       </c>
@@ -1234,7 +1255,7 @@
         <v>-119.271469</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>17</v>
       </c>
@@ -1245,7 +1266,7 @@
         <v>-122.484123</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>18</v>
       </c>
@@ -1256,7 +1277,7 @@
         <v>-118.394425</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>19</v>
       </c>
@@ -1267,7 +1288,7 @@
         <v>-118.463303</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>20</v>
       </c>
@@ -1278,7 +1299,7 @@
         <v>-122.419248</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>21</v>
       </c>
@@ -1289,7 +1310,7 @@
         <v>-123.810481</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>22</v>
       </c>
@@ -1300,7 +1321,7 @@
         <v>-117.174097</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>23</v>
       </c>
@@ -1311,7 +1332,7 @@
         <v>-118.184214</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>24</v>
       </c>
@@ -1322,7 +1343,7 @@
         <v>-118.101096</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>25</v>
       </c>
@@ -1333,7 +1354,7 @@
         <v>-118.247776</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>26</v>
       </c>
@@ -1344,7 +1365,7 @@
         <v>-118.321957</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>27</v>
       </c>
@@ -1355,7 +1376,7 @@
         <v>-124.349738</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>28</v>
       </c>
@@ -1366,7 +1387,7 @@
         <v>-117.231685</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>29</v>
       </c>
@@ -1377,7 +1398,7 @@
         <v>-118.463204</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>30</v>
       </c>
@@ -1388,7 +1409,7 @@
         <v>-124.08215199999999</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>31</v>
       </c>
@@ -1399,7 +1420,7 @@
         <v>-124.21766700000001</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>32</v>
       </c>
@@ -1410,7 +1431,7 @@
         <v>-122.32005100000001</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>33</v>
       </c>
@@ -1421,7 +1442,7 @@
         <v>-124.082708</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>34</v>
       </c>
@@ -1432,7 +1453,7 @@
         <v>-124.165243</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>35</v>
       </c>
@@ -1443,7 +1464,7 @@
         <v>-124.187217</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>36</v>
       </c>
@@ -1454,7 +1475,7 @@
         <v>-118.249933</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>37</v>
       </c>
@@ -1465,7 +1486,7 @@
         <v>-124.082083</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>38</v>
       </c>
@@ -1476,7 +1497,7 @@
         <v>-124.155423</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>39</v>
       </c>
@@ -1487,7 +1508,7 @@
         <v>-122.51463800000001</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>40</v>
       </c>
@@ -1498,7 +1519,7 @@
         <v>-120.740319</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>41</v>
       </c>
@@ -1509,7 +1530,7 @@
         <v>-120.868504</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>42</v>
       </c>
@@ -1520,7 +1541,7 @@
         <v>-117.234612</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>43</v>
       </c>
@@ -1531,7 +1552,7 @@
         <v>-122.59932999999999</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>44</v>
       </c>
@@ -1542,7 +1563,7 @@
         <v>-124.594556</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>45</v>
       </c>
@@ -1553,7 +1574,7 @@
         <v>-117.690687</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>46</v>
       </c>
@@ -1564,7 +1585,7 @@
         <v>-121.18243200000001</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>47</v>
       </c>
@@ -1575,7 +1596,7 @@
         <v>-124.241676</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>48</v>
       </c>
@@ -1586,7 +1607,7 @@
         <v>-123.958544</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>49</v>
       </c>
@@ -1597,7 +1618,7 @@
         <v>-122.49778000000001</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>50</v>
       </c>
@@ -1608,7 +1629,7 @@
         <v>-122.882335</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>51</v>
       </c>
@@ -1619,7 +1640,7 @@
         <v>-123.0508</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>52</v>
       </c>
@@ -1630,7 +1651,7 @@
         <v>-122.251278431914</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>53</v>
       </c>
@@ -1641,7 +1662,7 @@
         <v>-124.269088227574</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>54</v>
       </c>
@@ -1652,7 +1673,7 @@
         <v>-122.967399548244</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>55</v>
       </c>
@@ -1663,7 +1684,7 @@
         <v>-120.215035503311</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>56</v>
       </c>
@@ -1674,70 +1695,147 @@
         <v>-119.82889552341</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
+        <v>65</v>
+      </c>
+      <c r="B56" s="2">
+        <v>34.966440261044198</v>
+      </c>
+      <c r="C56" s="2">
+        <v>-120.657760310366</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A57" t="s">
         <v>57</v>
       </c>
-      <c r="B56" s="2">
+      <c r="B57" s="2">
         <v>46.551366786857699</v>
       </c>
-      <c r="C56" s="2">
+      <c r="C57" s="2">
         <v>-123.992817460175</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A57" t="s">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A58" t="s">
         <v>59</v>
       </c>
-      <c r="B57" s="2">
+      <c r="B58" s="2">
         <v>40.767722999999997</v>
       </c>
-      <c r="C57" s="2">
+      <c r="C58" s="2">
         <v>-124.241676</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A58" s="1" t="s">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A59" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B58" s="2">
+      <c r="B59" s="2">
         <v>37.499510997959497</v>
       </c>
-      <c r="C58" s="2">
+      <c r="C59" s="2">
         <v>-122.199083685142</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A59" t="s">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A60" t="s">
         <v>60</v>
       </c>
-      <c r="B59" s="2">
+      <c r="B60" s="2">
         <v>35.6428757415744</v>
       </c>
-      <c r="C59" s="2">
+      <c r="C60" s="2">
         <v>-121.187654767788</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A60" t="s">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A61" t="s">
         <v>61</v>
       </c>
-      <c r="B60" s="2">
+      <c r="B61" s="2">
         <v>47.266223226637102</v>
       </c>
-      <c r="C60" s="2">
+      <c r="C61" s="2">
         <v>-122.412717792104</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A61" t="s">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A62" t="s">
         <v>62</v>
       </c>
-      <c r="B61" s="2">
+      <c r="B62" s="2">
         <v>48.010603159705703</v>
       </c>
-      <c r="C61" s="2">
+      <c r="C62" s="2">
         <v>-122.443289771696</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A63" t="s">
+        <v>63</v>
+      </c>
+      <c r="B63" s="2">
+        <v>46.259540000000001</v>
+      </c>
+      <c r="C63" s="2">
+        <v>-124.082083</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A64" t="s">
+        <v>64</v>
+      </c>
+      <c r="B64" s="2">
+        <v>40.727520494834501</v>
+      </c>
+      <c r="C64" s="2">
+        <v>-124.22085681388</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A65" t="s">
+        <v>66</v>
+      </c>
+      <c r="B65" s="2">
+        <v>38.143129512729601</v>
+      </c>
+      <c r="C65" s="2">
+        <v>-122.88032128675</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A66" t="s">
+        <v>67</v>
+      </c>
+      <c r="B66" s="2">
+        <v>42.738932436794897</v>
+      </c>
+      <c r="C66" s="2">
+        <v>-124.49862438502601</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A67" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B67" s="2">
+        <v>38.089187955173301</v>
+      </c>
+      <c r="C67" s="2">
+        <v>-122.29490950278699</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A68" t="s">
+        <v>69</v>
+      </c>
+      <c r="B68" s="2">
+        <v>36.622672000000001</v>
+      </c>
+      <c r="C68" s="2">
+        <v>-121.885687</v>
       </c>
     </row>
   </sheetData>

</xml_diff>